<commit_message>
Atualização mês de Abril de 2021.
</commit_message>
<xml_diff>
--- a/data/free_float/base_free_float.xlsx
+++ b/data/free_float/base_free_float.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a548da2118d25344/Alysson/Unifor/Monitoria/indice_nupe/data/free_float/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{A902C639-3340-449C-A368-F1A6E7D1F3FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6BFBDBFC-A028-4FCE-92E2-AA1AB4C1AB36}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{A902C639-3340-449C-A368-F1A6E7D1F3FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D358613D-1BDD-4808-A56A-415358EC4C1F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B356B7D1-A110-4F9A-A775-3A3350BF201E}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B356B7D1-A110-4F9A-A775-3A3350BF201E}"/>
   </bookViews>
   <sheets>
     <sheet name="tickers" sheetId="1" r:id="rId1"/>
@@ -70,8 +70,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -128,7 +131,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -138,6 +141,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3373347B-3080-4674-8742-48133809A55D}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,8 +476,10 @@
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -577,8 +586,27 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M5" s="5"/>
     </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H9" s="7"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H10" s="9"/>
+    </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I12" s="8"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="8"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K2:K10">

</xml_diff>

<commit_message>
Ajustando free-float das empresas
Para finalizar o script é preciso ajustar a quantidade de ações pegas no site da CVM dentro do código.

Na próxima versão será abolido o uso do pacote batchgetsymbols por conta de sua baica qualidade na obtenção das informações do preço das ações.
</commit_message>
<xml_diff>
--- a/data/free_float/base_free_float.xlsx
+++ b/data/free_float/base_free_float.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a548da2118d25344/Alysson/Unifor/Monitoria/indice_nupe/data/free_float/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alyss\OneDrive\Alysson\Unifor\Monitoria\indice_nupe\data\free_float\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{A902C639-3340-449C-A368-F1A6E7D1F3FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D358613D-1BDD-4808-A56A-415358EC4C1F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D144473-A6DC-47D0-8D53-42B612DF03E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B356B7D1-A110-4F9A-A775-3A3350BF201E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B356B7D1-A110-4F9A-A775-3A3350BF201E}"/>
   </bookViews>
   <sheets>
     <sheet name="tickers" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -141,10 +141,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,10 +477,10 @@
     <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -581,10 +581,43 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44307</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.28459279237716756</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.99655525055169814</v>
+      </c>
+      <c r="D4" s="3">
+        <v>7.1112723063256169E-3</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2.0880696419320013E-2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.64453280555693382</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.29747625698324021</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.32864406481746694</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.24681351622418879</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.35900134918330517</v>
+      </c>
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M5" s="5"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H8" s="7"/>
@@ -593,11 +626,14 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H9" s="7"/>
       <c r="I9" s="8"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Atualização do Índice - 12/09/2021
</commit_message>
<xml_diff>
--- a/data/free_float/base_free_float.xlsx
+++ b/data/free_float/base_free_float.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alyss\OneDrive\Alysson\Unifor\Monitoria\indice_nupe\data\free_float\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a548da2118d25344/Alysson/Unifor/Monitoria/indice_nupe/data/free_float/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCDAB2D-B4EB-44B0-8E79-E0EAB56C9E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{7BCDAB2D-B4EB-44B0-8E79-E0EAB56C9E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4FE5C37-FE91-4E4E-B14D-60FEF5BF255D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B356B7D1-A110-4F9A-A775-3A3350BF201E}"/>
   </bookViews>
@@ -73,12 +73,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -149,11 +148,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,7 +474,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +523,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -560,7 +559,7 @@
         <v>0.35900134918330517</v>
       </c>
       <c r="K2" s="12">
-        <v>0.2</v>
+        <v>0.19995517161454573</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -595,7 +594,7 @@
         <v>0.35900134918330517</v>
       </c>
       <c r="K3" s="12">
-        <v>0.2</v>
+        <v>0.19995517161454573</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -630,7 +629,7 @@
         <v>0.35900134918330517</v>
       </c>
       <c r="K4" s="12">
-        <v>0.2</v>
+        <v>0.19995517161454573</v>
       </c>
       <c r="M4" s="4"/>
     </row>
@@ -666,7 +665,7 @@
         <v>0.35900134918330517</v>
       </c>
       <c r="K5" s="12">
-        <v>0.2</v>
+        <v>0.19995517161454573</v>
       </c>
       <c r="M5" s="5"/>
     </row>
@@ -702,7 +701,7 @@
         <v>0.35900134918330517</v>
       </c>
       <c r="K6" s="12">
-        <v>0.2</v>
+        <v>0.19995517161454573</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -716,7 +715,7 @@
         <v>0.99655525055169814</v>
       </c>
       <c r="D7" s="3">
-        <v>7.1112723063256169E-3</v>
+        <v>7.1114575526935609E-3</v>
       </c>
       <c r="E7" s="3">
         <v>2.0880696419320013E-2</v>
@@ -731,13 +730,13 @@
         <v>0.32864406481746694</v>
       </c>
       <c r="I7" s="3">
-        <v>0.24681351622418879</v>
+        <v>0.24533693805309734</v>
       </c>
       <c r="J7" s="3">
-        <v>0.35900134918330517</v>
+        <v>0.35567808885003749</v>
       </c>
       <c r="K7" s="12">
-        <v>0.2</v>
+        <v>0.19995517161454573</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -754,8 +753,9 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J11" s="8"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="11"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I12" s="8"/>

</xml_diff>